<commit_message>
file ann  bert csv xlsl
</commit_message>
<xml_diff>
--- a/annotazione/martyna_piotrowicz.xlsx
+++ b/annotazione/martyna_piotrowicz.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wierz\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gretagorzoni/Desktop/Semantica2025/annotazione/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2183666E-F6E6-4574-B1D6-2AA7419DFDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9EB8E58-DF78-DC49-AEEB-EEE125BDC849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8E7A6423-0A15-F74D-9B2B-336A86706306}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{8E7A6423-0A15-F74D-9B2B-336A86706306}"/>
   </bookViews>
   <sheets>
     <sheet name="esperimento" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="251">
   <si>
     <t>ID</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>E poi magari la madre va via piangendo a tutto spiano ma almeno l'ha abbracciata, ha saputo che sta bene: viso</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>viso .</t>
@@ -1231,15 +1228,15 @@
       <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="80.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1253,7 +1250,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>41</v>
       </c>
@@ -1261,1676 +1258,1676 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>87</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>113</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>108</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>65</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>67</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>58</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>80</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>74</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>47</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>39</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>118</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>28</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>33</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>104</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>97</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>18</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>102</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>12</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>116</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>48</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>17</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>95</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>103</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>73</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>79</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>90</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>70</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>98</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>31</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>114</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>66</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>83</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>27</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>56</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>30</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>89</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>81</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>51</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>29</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>107</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>86</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>46</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>45</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>32</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>53</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>72</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>26</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>38</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>100</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>36</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>22</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>111</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>7</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>85</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>5</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>25</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>76</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>84</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>50</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>57</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>78</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>82</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>63</v>
       </c>
       <c r="B75" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>61</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="78" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>59</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>62</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>44</v>
       </c>
       <c r="B79" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>112</v>
       </c>
       <c r="B80" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>75</v>
       </c>
       <c r="B81" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>54</v>
       </c>
       <c r="B82" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>77</v>
       </c>
       <c r="B83" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>94</v>
       </c>
       <c r="B84" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>91</v>
       </c>
       <c r="B85" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>93</v>
       </c>
       <c r="B86" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>49</v>
       </c>
       <c r="B87" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>105</v>
       </c>
       <c r="B88" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>109</v>
       </c>
       <c r="B89" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>71</v>
       </c>
       <c r="B90" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>8</v>
       </c>
       <c r="B91" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>110</v>
       </c>
       <c r="B92" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D92" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>2</v>
       </c>
       <c r="B93" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C93" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>101</v>
       </c>
       <c r="B94" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D94" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>106</v>
       </c>
       <c r="B95" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D95" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>16</v>
       </c>
       <c r="B96" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C96" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>119</v>
       </c>
       <c r="B97" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>4</v>
       </c>
       <c r="B98" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>14</v>
       </c>
       <c r="B99" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C99" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="100" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>15</v>
       </c>
       <c r="B100" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D100" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="101" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>20</v>
       </c>
       <c r="B101" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>19</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="103" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>69</v>
       </c>
       <c r="B103" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C103" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="104" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>52</v>
       </c>
       <c r="B104" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C104" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>115</v>
       </c>
       <c r="B105" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C105" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>34</v>
       </c>
       <c r="B106" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D106" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="107" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>99</v>
       </c>
       <c r="B107" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D107" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C107" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="108" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>88</v>
       </c>
       <c r="B108" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D108" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="109" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>37</v>
       </c>
       <c r="B109" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D109" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="110" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>35</v>
       </c>
       <c r="B110" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D110" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="111" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>96</v>
       </c>
       <c r="B111" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D111" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C111" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="112" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>40</v>
       </c>
       <c r="B112" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D112" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C112" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="113" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>9</v>
       </c>
       <c r="B113" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C113" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="114" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>0</v>
       </c>
       <c r="B114" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D114" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C114" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="115" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>92</v>
       </c>
       <c r="B115" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D115" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C115" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="116" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>60</v>
       </c>
       <c r="B116" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D116" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C116" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="117" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>68</v>
       </c>
       <c r="B117" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D117" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C117" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="118" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>117</v>
       </c>
       <c r="B118" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D118" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="C118" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="119" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>10</v>
       </c>
       <c r="B119" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D119" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C119" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="120" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>55</v>
       </c>
       <c r="B120" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D120" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C120" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="121" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>64</v>
       </c>
       <c r="B121" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D121" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2942,6 +2939,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9CED8EAC5CDC4469EF7330F25FDB9A3" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1cee761af582467ca71230ca55e67b32">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="faf19e63-e5c2-49de-ad4c-b78cf1af40cf" xmlns:ns4="b6699f54-5d2b-4cb0-9fc8-f39dea529984" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="61ca80d820cc91cb5c9c72f7b9e49aec" ns3:_="" ns4:_="">
     <xsd:import namespace="faf19e63-e5c2-49de-ad4c-b78cf1af40cf"/>
@@ -3162,15 +3168,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3180,6 +3177,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{630D69B0-5A49-441C-B9FA-E8A92072B9A5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6582BD4C-ED30-44F1-816D-1B9ECCCD321D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3194,14 +3199,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{630D69B0-5A49-441C-B9FA-E8A92072B9A5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>